<commit_message>
Ahora si que doy mucha informacion
</commit_message>
<xml_diff>
--- a/TestAutomataDFA_NFA/ResultadosFinal/RepCiberia.dot_CONTINUO_877371829432085.xlsx
+++ b/TestAutomataDFA_NFA/ResultadosFinal/RepCiberia.dot_CONTINUO_877371829432085.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27630" windowHeight="11340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27630" windowHeight="11340" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Construccion_Navegacion" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="NavegacionNFA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1:AB35"/>
+  <oleSize ref="AQ25:BQ59"/>
 </workbook>
 </file>
 
@@ -6279,11 +6279,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="422064104"/>
-        <c:axId val="422064496"/>
+        <c:axId val="419616640"/>
+        <c:axId val="419620952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="422064104"/>
+        <c:axId val="419616640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6325,7 +6325,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422064496"/>
+        <c:crossAx val="419620952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6333,7 +6333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422064496"/>
+        <c:axId val="419620952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6384,7 +6384,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422064104"/>
+        <c:crossAx val="419616640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6505,7 +6505,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6972,11 +6971,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="419713632"/>
-        <c:axId val="419716376"/>
+        <c:axId val="419617424"/>
+        <c:axId val="419621344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="419713632"/>
+        <c:axId val="419617424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7013,7 +7012,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7079,7 +7077,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419716376"/>
+        <c:crossAx val="419621344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7087,7 +7085,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419716376"/>
+        <c:axId val="419621344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7133,7 +7131,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7194,7 +7191,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419713632"/>
+        <c:crossAx val="419617424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7208,7 +7205,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7315,7 +7311,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7782,11 +7777,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="476593688"/>
-        <c:axId val="476592904"/>
+        <c:axId val="419620168"/>
+        <c:axId val="419617816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="476593688"/>
+        <c:axId val="419620168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7818,7 +7813,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7884,7 +7878,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476592904"/>
+        <c:crossAx val="419617816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7892,7 +7886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="476592904"/>
+        <c:axId val="419617816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7943,7 +7937,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8004,7 +7997,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476593688"/>
+        <c:crossAx val="419620168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8018,7 +8011,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8917,11 +8909,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="489073664"/>
-        <c:axId val="489071312"/>
+        <c:axId val="384378280"/>
+        <c:axId val="423376008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="489073664"/>
+        <c:axId val="384378280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8964,7 +8956,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489071312"/>
+        <c:crossAx val="423376008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8972,7 +8964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="489071312"/>
+        <c:axId val="423376008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9023,7 +9015,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489073664"/>
+        <c:crossAx val="384378280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11728,7 +11720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
@@ -45388,8 +45380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:MJ59"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BQ49" sqref="BQ49"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AZ1" sqref="AZ1:AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>